<commit_message>
cleaned up until Template 7
</commit_message>
<xml_diff>
--- a/i_codebooks/D4_DU_matched_MS-PREGNANCY-COHORT_to_MS-COHORT.xlsx
+++ b/i_codebooks/D4_DU_matched_MS-PREGNANCY-COHORT_to_MS-COHORT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -320,20 +320,20 @@
     <t>end_preg_period_pre_all_MS_pregnancy_id</t>
   </si>
   <si>
-    <t>is_pregnant</t>
-  </si>
-  <si>
     <t>0 = MS pregnancy
 1 = MS matched non pregnant</t>
-  </si>
-  <si>
-    <t>0 = MS pregnancy</t>
   </si>
   <si>
     <t>1 = first non-pregnant MS</t>
   </si>
   <si>
     <t>binary variable identifying whether the record is about a true pregnancy or a matched equal pregnancy</t>
+  </si>
+  <si>
+    <t>is_pregnancy</t>
+  </si>
+  <si>
+    <t>binary</t>
   </si>
 </sst>
 </file>
@@ -343,7 +343,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,22 +361,33 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF444444"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -387,6 +398,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -394,11 +406,13 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -580,82 +594,82 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -665,6 +679,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -882,7 +897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -3954,11 +3969,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K956"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -4048,16 +4063,16 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="A6" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="38" t="s">
         <v>96</v>
-      </c>
-      <c r="B6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
@@ -4068,7 +4083,7 @@
         <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">

</xml_diff>